<commit_message>
add a new feature i18n
</commit_message>
<xml_diff>
--- a/blanco-meta/telegrams/RequestHeader.xlsx
+++ b/blanco-meta/telegrams/RequestHeader.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10520"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuji/projects/dapanda/dapanda-api-core/blanco-meta/telegrams/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00439FFA-BC65-144D-A48C-C990425DA31F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{174F1790-A3F6-D949-9BB3-508B4FE82C73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="78">
   <si>
     <t>クラス名</t>
   </si>
@@ -482,6 +482,14 @@
   </si>
   <si>
     <t>null</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>lang</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>言語コード</t>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -1171,6 +1179,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1194,21 +1217,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1626,8 +1634,8 @@
   </sheetPr>
   <dimension ref="A1:AA61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1769,10 +1777,10 @@
       <c r="U8" s="54"/>
     </row>
     <row r="9" spans="1:22" s="15" customFormat="1">
-      <c r="A9" s="92" t="s">
+      <c r="A9" s="97" t="s">
         <v>50</v>
       </c>
-      <c r="B9" s="93"/>
+      <c r="B9" s="98"/>
       <c r="C9" s="61" t="s">
         <v>51</v>
       </c>
@@ -1815,10 +1823,10 @@
         <v>69</v>
       </c>
       <c r="B12" s="35"/>
-      <c r="C12" s="101"/>
-      <c r="D12" s="102"/>
-      <c r="E12" s="102"/>
-      <c r="F12" s="103"/>
+      <c r="C12" s="93"/>
+      <c r="D12" s="94"/>
+      <c r="E12" s="94"/>
+      <c r="F12" s="95"/>
     </row>
     <row r="13" spans="1:22">
       <c r="A13" s="3" t="s">
@@ -2538,83 +2546,83 @@
       <c r="W44" s="67"/>
     </row>
     <row r="45" spans="1:27" ht="13.5" customHeight="1">
-      <c r="A45" s="95" t="s">
+      <c r="A45" s="100" t="s">
         <v>4</v>
       </c>
-      <c r="B45" s="95" t="s">
+      <c r="B45" s="100" t="s">
         <v>5</v>
       </c>
-      <c r="C45" s="94" t="s">
+      <c r="C45" s="99" t="s">
         <v>6</v>
       </c>
-      <c r="D45" s="94" t="s">
+      <c r="D45" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="E45" s="96" t="s">
+      <c r="E45" s="101" t="s">
         <v>16</v>
       </c>
-      <c r="F45" s="94" t="s">
+      <c r="F45" s="99" t="s">
         <v>7</v>
       </c>
-      <c r="G45" s="98" t="s">
+      <c r="G45" s="103" t="s">
         <v>49</v>
       </c>
-      <c r="H45" s="100" t="s">
+      <c r="H45" s="92" t="s">
         <v>62</v>
       </c>
-      <c r="I45" s="100" t="s">
+      <c r="I45" s="92" t="s">
         <v>63</v>
       </c>
-      <c r="J45" s="100" t="s">
+      <c r="J45" s="92" t="s">
         <v>64</v>
       </c>
-      <c r="K45" s="100" t="s">
+      <c r="K45" s="92" t="s">
         <v>65</v>
       </c>
-      <c r="L45" s="100" t="s">
+      <c r="L45" s="92" t="s">
         <v>66</v>
       </c>
-      <c r="M45" s="99" t="s">
+      <c r="M45" s="104" t="s">
         <v>67</v>
       </c>
-      <c r="N45" s="99" t="s">
+      <c r="N45" s="104" t="s">
         <v>68</v>
       </c>
-      <c r="O45" s="97" t="s">
+      <c r="O45" s="102" t="s">
         <v>17</v>
       </c>
-      <c r="P45" s="97"/>
-      <c r="Q45" s="97" t="s">
+      <c r="P45" s="102"/>
+      <c r="Q45" s="102" t="s">
         <v>18</v>
       </c>
-      <c r="R45" s="97"/>
+      <c r="R45" s="102"/>
       <c r="S45" s="72" t="s">
         <v>19</v>
       </c>
-      <c r="T45" s="94" t="s">
+      <c r="T45" s="99" t="s">
         <v>2</v>
       </c>
-      <c r="U45" s="94"/>
-      <c r="V45" s="104" t="s">
+      <c r="U45" s="99"/>
+      <c r="V45" s="96" t="s">
         <v>71</v>
       </c>
       <c r="W45" s="67"/>
     </row>
     <row r="46" spans="1:27">
-      <c r="A46" s="95"/>
-      <c r="B46" s="95"/>
-      <c r="C46" s="94"/>
-      <c r="D46" s="94"/>
-      <c r="E46" s="96"/>
-      <c r="F46" s="94"/>
-      <c r="G46" s="98"/>
-      <c r="H46" s="100"/>
-      <c r="I46" s="100"/>
-      <c r="J46" s="100"/>
-      <c r="K46" s="100"/>
-      <c r="L46" s="100"/>
-      <c r="M46" s="99"/>
-      <c r="N46" s="99"/>
+      <c r="A46" s="100"/>
+      <c r="B46" s="100"/>
+      <c r="C46" s="99"/>
+      <c r="D46" s="99"/>
+      <c r="E46" s="101"/>
+      <c r="F46" s="99"/>
+      <c r="G46" s="103"/>
+      <c r="H46" s="92"/>
+      <c r="I46" s="92"/>
+      <c r="J46" s="92"/>
+      <c r="K46" s="92"/>
+      <c r="L46" s="92"/>
+      <c r="M46" s="104"/>
+      <c r="N46" s="104"/>
       <c r="O46" s="73" t="s">
         <v>20</v>
       </c>
@@ -2630,9 +2638,9 @@
       <c r="S46" s="73" t="s">
         <v>24</v>
       </c>
-      <c r="T46" s="94"/>
-      <c r="U46" s="94"/>
-      <c r="V46" s="104"/>
+      <c r="T46" s="99"/>
+      <c r="U46" s="99"/>
+      <c r="V46" s="96"/>
       <c r="W46" s="67"/>
     </row>
     <row r="47" spans="1:27">
@@ -2677,12 +2685,20 @@
         <f>A47+1</f>
         <v>2</v>
       </c>
-      <c r="B48" s="75"/>
-      <c r="C48" s="76"/>
+      <c r="B48" s="75" t="s">
+        <v>76</v>
+      </c>
+      <c r="C48" s="76" t="s">
+        <v>73</v>
+      </c>
       <c r="D48" s="76"/>
       <c r="E48" s="77"/>
-      <c r="F48" s="76"/>
-      <c r="G48" s="78"/>
+      <c r="F48" s="76" t="s">
+        <v>75</v>
+      </c>
+      <c r="G48" s="78" t="s">
+        <v>37</v>
+      </c>
       <c r="H48" s="76"/>
       <c r="I48" s="79"/>
       <c r="J48" s="79"/>
@@ -2697,7 +2713,9 @@
       <c r="S48" s="76"/>
       <c r="T48" s="76"/>
       <c r="U48" s="80"/>
-      <c r="V48" s="79"/>
+      <c r="V48" s="79" t="s">
+        <v>77</v>
+      </c>
       <c r="W48" s="67"/>
     </row>
     <row r="49" spans="1:23">
@@ -3031,6 +3049,10 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="N45:N46"/>
+    <mergeCell ref="H45:H46"/>
+    <mergeCell ref="I45:I46"/>
+    <mergeCell ref="J45:J46"/>
     <mergeCell ref="K45:K46"/>
     <mergeCell ref="C12:F12"/>
     <mergeCell ref="V45:V46"/>
@@ -3047,10 +3069,6 @@
     <mergeCell ref="Q45:R45"/>
     <mergeCell ref="G45:G46"/>
     <mergeCell ref="M45:M46"/>
-    <mergeCell ref="N45:N46"/>
-    <mergeCell ref="H45:H46"/>
-    <mergeCell ref="I45:I46"/>
-    <mergeCell ref="J45:J46"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <dataValidations count="7">

</xml_diff>

<commit_message>
kapt3 not permit generic definition of final class.
</commit_message>
<xml_diff>
--- a/blanco-meta/telegrams/RequestHeader.xlsx
+++ b/blanco-meta/telegrams/RequestHeader.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10714"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/dapanda/dapanda-api-core/blanco-meta/telegrams/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E049188-70C4-6347-ABC8-85302F55B9C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60CAA695-75DF-5C4A-AAF9-C26A45BA8A2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4100" yWindow="900" windowWidth="24700" windowHeight="17100" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="80">
   <si>
     <t>クラス名</t>
   </si>
@@ -1839,7 +1839,7 @@
   <dimension ref="A1:Y51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -2019,9 +2019,7 @@
         <v>69</v>
       </c>
       <c r="B15" s="12"/>
-      <c r="C15" s="51" t="s">
-        <v>38</v>
-      </c>
+      <c r="C15" s="51"/>
       <c r="D15" t="s">
         <v>70</v>
       </c>
@@ -2081,9 +2079,7 @@
         <v>72</v>
       </c>
       <c r="B17" s="12"/>
-      <c r="C17" s="51" t="s">
-        <v>38</v>
-      </c>
+      <c r="C17" s="51"/>
       <c r="D17"/>
       <c r="E17"/>
       <c r="F17"/>

</xml_diff>